<commit_message>
Implementa suporte para múltiplas abas no processamento de planilhas Excel, adicionando a aba "Ações" e atualizando a aba "Consolidado". Inclui visualização detalhada da carteira de ações na interface e atualiza a documentação no README.
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dti\FinancasPessoais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE8467E-8489-43BE-AB9B-7EA1840D8284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5245CD0C-31F4-409F-AC0E-3DF7159FE9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Consolidado" sheetId="1" r:id="rId1"/>
+    <sheet name="Ações" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="116">
   <si>
     <t>Alias</t>
   </si>
@@ -204,6 +205,186 @@
   </si>
   <si>
     <t>Previdência Privada</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Renda Esperada</t>
+  </si>
+  <si>
+    <t>Capital Atual</t>
+  </si>
+  <si>
+    <t>Dividend Yield Esperado</t>
+  </si>
+  <si>
+    <t>Dividend Yield Pago</t>
+  </si>
+  <si>
+    <t>Proporção Hoje</t>
+  </si>
+  <si>
+    <t>Meta 28k</t>
+  </si>
+  <si>
+    <t>Meta +1.a.</t>
+  </si>
+  <si>
+    <t>Meta qtd. 2033</t>
+  </si>
+  <si>
+    <t>BBAS3</t>
+  </si>
+  <si>
+    <t>R$1.10</t>
+  </si>
+  <si>
+    <t>R$5,558.31</t>
+  </si>
+  <si>
+    <t>R$104,014.05</t>
+  </si>
+  <si>
+    <t>R$5,302.45</t>
+  </si>
+  <si>
+    <t>BBSE3</t>
+  </si>
+  <si>
+    <t>R$3.81</t>
+  </si>
+  <si>
+    <t>R$12,261.52</t>
+  </si>
+  <si>
+    <t>R$105,583.80</t>
+  </si>
+  <si>
+    <t>R$7,316.81</t>
+  </si>
+  <si>
+    <t>BRSR6</t>
+  </si>
+  <si>
+    <t>R$1,445.81</t>
+  </si>
+  <si>
+    <t>R$15,531.48</t>
+  </si>
+  <si>
+    <t>R$692.74</t>
+  </si>
+  <si>
+    <t>CEBR6</t>
+  </si>
+  <si>
+    <t>R$2.29</t>
+  </si>
+  <si>
+    <t>R$1,476.44</t>
+  </si>
+  <si>
+    <t>R$15,480.00</t>
+  </si>
+  <si>
+    <t>R$815.67</t>
+  </si>
+  <si>
+    <t>CXSE3</t>
+  </si>
+  <si>
+    <t>R$1.32</t>
+  </si>
+  <si>
+    <t>R$1,861.20</t>
+  </si>
+  <si>
+    <t>R$19,204.20</t>
+  </si>
+  <si>
+    <t>R$1,325.40</t>
+  </si>
+  <si>
+    <t>LEVE3</t>
+  </si>
+  <si>
+    <t>R$2.74</t>
+  </si>
+  <si>
+    <t>R$1,735.40</t>
+  </si>
+  <si>
+    <t>R$17,396.96</t>
+  </si>
+  <si>
+    <t>R$1,329.75</t>
+  </si>
+  <si>
+    <t>PETR4</t>
+  </si>
+  <si>
+    <t>R$2.97</t>
+  </si>
+  <si>
+    <t>R$857.67</t>
+  </si>
+  <si>
+    <t>R$8,719.13</t>
+  </si>
+  <si>
+    <t>R$588.92</t>
+  </si>
+  <si>
+    <t>RANI3</t>
+  </si>
+  <si>
+    <t>R$0.76</t>
+  </si>
+  <si>
+    <t>R$1,109.61</t>
+  </si>
+  <si>
+    <t>R$10,818.60</t>
+  </si>
+  <si>
+    <t>R$845.49</t>
+  </si>
+  <si>
+    <t>ISAE4</t>
+  </si>
+  <si>
+    <t>R$1.59</t>
+  </si>
+  <si>
+    <t>R$790.43</t>
+  </si>
+  <si>
+    <t>R$10,976.48</t>
+  </si>
+  <si>
+    <t>R$1,170.91</t>
+  </si>
+  <si>
+    <t>CGAS5</t>
+  </si>
+  <si>
+    <t>R$10.56</t>
+  </si>
+  <si>
+    <t>R$137.34</t>
+  </si>
+  <si>
+    <t>R$1,664.00</t>
+  </si>
+  <si>
+    <t>R$9.95</t>
+  </si>
+  <si>
+    <t>Div. Esperado 2025</t>
+  </si>
+  <si>
+    <t>Qtd</t>
   </si>
 </sst>
 </file>
@@ -239,8 +420,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,11 +709,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:N33"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,4 +1714,417 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87E23EC-653B-4EE1-A707-56B5CDB99AAE}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>5037</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.3362</v>
+      </c>
+      <c r="I2">
+        <v>-142</v>
+      </c>
+      <c r="J2" s="3">
+        <v>-2519</v>
+      </c>
+      <c r="K2" s="3">
+        <v>-45417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>3220</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.11609999999999999</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.34129999999999999</v>
+      </c>
+      <c r="I3">
+        <v>-91</v>
+      </c>
+      <c r="J3" s="3">
+        <v>-1610</v>
+      </c>
+      <c r="K3" s="3">
+        <v>-29034</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4">
+        <v>1314</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="2">
+        <v>9.3100000000000002E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5.0200000000000002E-2</v>
+      </c>
+      <c r="I4">
+        <v>-37</v>
+      </c>
+      <c r="J4">
+        <v>-657</v>
+      </c>
+      <c r="K4" s="3">
+        <v>-11848</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
+        <v>645</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9.5399999999999999E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <v>-18</v>
+      </c>
+      <c r="J5">
+        <v>-323</v>
+      </c>
+      <c r="K5" s="3">
+        <v>-5816</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6">
+        <v>1410</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="2">
+        <v>9.69E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="2">
+        <v>6.2100000000000002E-2</v>
+      </c>
+      <c r="I6">
+        <v>-40</v>
+      </c>
+      <c r="J6">
+        <v>-705</v>
+      </c>
+      <c r="K6" s="3">
+        <v>-12714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7">
+        <v>634</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="2">
+        <v>9.98E-2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5.62E-2</v>
+      </c>
+      <c r="I7">
+        <v>-18</v>
+      </c>
+      <c r="J7">
+        <v>-317</v>
+      </c>
+      <c r="K7" s="3">
+        <v>-5717</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8">
+        <v>289</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="2">
+        <v>9.8400000000000001E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>-8</v>
+      </c>
+      <c r="J8">
+        <v>-145</v>
+      </c>
+      <c r="K8" s="3">
+        <v>-2606</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9">
+        <v>1460</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.1026</v>
+      </c>
+      <c r="G9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I9">
+        <v>-41</v>
+      </c>
+      <c r="J9">
+        <v>-730</v>
+      </c>
+      <c r="K9" s="3">
+        <v>-13164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10">
+        <v>496</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="2">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="I10">
+        <v>-14</v>
+      </c>
+      <c r="J10">
+        <v>-248</v>
+      </c>
+      <c r="K10" s="3">
+        <v>-4472</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="2">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>-7</v>
+      </c>
+      <c r="K11">
+        <v>-117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>